<commit_message>
Inventory Management - Add Z Transfer Posting and Z Good Issue to Production
</commit_message>
<xml_diff>
--- a/im/media/template/template_material.xlsx
+++ b/im/media/template/template_material.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Material Type (4)</t>
   </si>
   <si>
+    <t>Material Group (20)</t>
+  </si>
+  <si>
     <t>Material Number (40)</t>
   </si>
   <si>
@@ -38,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">FIN = Finished Goods, RAW = Raw Material </t>
+  </si>
+  <si>
+    <t>Material Group</t>
+  </si>
+  <si>
+    <t>RAW = Raw Material, E11 = ASMP01, E12 = ASIPP01, E13 = ASVP01, E15 = ASANP01</t>
   </si>
   <si>
     <t>Material Number</t>
@@ -69,9 +78,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
@@ -113,8 +122,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -152,16 +169,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -175,9 +184,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,6 +200,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -215,13 +231,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -229,7 +238,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,6 +259,144 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -262,31 +409,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,139 +427,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,6 +464,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -510,30 +534,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -551,6 +551,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -561,18 +570,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -582,127 +591,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1038,24 +1047,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="16.7777777777778" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1111111111111" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.2222222222222" customWidth="1"/>
-    <col min="9" max="9" width="61.6666666666667" customWidth="1"/>
+    <col min="2" max="3" width="21" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1111111111111" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.2222222222222" customWidth="1"/>
+    <col min="10" max="10" width="75.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1071,51 +1080,62 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="8:9">
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1"/>
+    <row r="2" spans="9:10">
+      <c r="I2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="8:9">
-      <c r="H3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="1" t="s">
+    <row r="3" spans="9:10">
+      <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="8:9">
-      <c r="H4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="1" t="s">
+    <row r="4" spans="9:10">
+      <c r="I4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="8:9">
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1" t="s">
+    <row r="5" spans="9:10">
+      <c r="I5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="8:9">
-      <c r="H6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1" t="s">
+    <row r="6" spans="9:10">
+      <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="7" spans="8:9">
-      <c r="H7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="1" t="s">
+    <row r="7" spans="9:10">
+      <c r="I7" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="9:10">
+      <c r="I8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>